<commit_message>
concrate test cases was created to develop, user decice SAT on console
</commit_message>
<xml_diff>
--- a/SoftwareTestingTermProject/Output/Homework1_template.xlsx
+++ b/SoftwareTestingTermProject/Output/Homework1_template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0" showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView activeTab="5" firstSheet="3" tabRatio="500" windowHeight="6810" windowWidth="10305" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
-    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="Input Variables" sheetId="2" r:id="rId2"/>
-    <sheet name="Output Variables" sheetId="8" r:id="rId3"/>
-    <sheet name="Conditions" sheetId="3" r:id="rId4"/>
-    <sheet name="Actions" sheetId="4" r:id="rId5"/>
-    <sheet name="Decision Table" sheetId="5" r:id="rId6"/>
-    <sheet name="Abstract Test Cases" sheetId="6" r:id="rId7"/>
-    <sheet name="Concrete Test Cases" sheetId="7" r:id="rId8"/>
+    <sheet name="Requirements" r:id="rId1" sheetId="1"/>
+    <sheet name="Input Variables" r:id="rId2" sheetId="2"/>
+    <sheet name="Output Variables" r:id="rId3" sheetId="8"/>
+    <sheet name="Conditions" r:id="rId4" sheetId="3"/>
+    <sheet name="Actions" r:id="rId5" sheetId="4"/>
+    <sheet name="Decision Table" r:id="rId6" sheetId="5"/>
+    <sheet name="Abstract Test Cases" r:id="rId7" sheetId="6"/>
+    <sheet name="Concrete Test Cases" r:id="rId8" sheetId="7"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <oleSize ref="A1:F20"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="74">
   <si>
     <t>Requirements</t>
   </si>
@@ -187,12 +188,6 @@
     <t>type_of_triangle="Isosceles"</t>
   </si>
   <si>
-    <t>Equaliteral</t>
-  </si>
-  <si>
-    <t>Impossible</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -200,13 +195,68 @@
   </si>
   <si>
     <t>R5</t>
+  </si>
+  <si>
+    <t>type_of_triangle="Equaliteral"</t>
+  </si>
+  <si>
+    <t>type_of_triangle="Impossible"</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>ATC3</t>
+  </si>
+  <si>
+    <t>ATC4</t>
+  </si>
+  <si>
+    <t>ATC5</t>
+  </si>
+  <si>
+    <t>ATC6</t>
+  </si>
+  <si>
+    <t>ATC7</t>
+  </si>
+  <si>
+    <t>ATC8</t>
+  </si>
+  <si>
+    <t>ATC9</t>
+  </si>
+  <si>
+    <t>ATC10</t>
+  </si>
+  <si>
+    <t>ATC11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,42 +314,45 @@
     </border>
   </borders>
   <cellStyleXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="8">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="4"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="6"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="3"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -313,10 +366,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -470,7 +523,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -479,13 +532,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -495,7 +548,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -504,7 +557,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -513,7 +566,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -523,12 +576,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -559,7 +612,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -578,7 +631,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -629,23 +682,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -653,13 +706,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -669,24 +722,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -694,7 +747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -702,7 +755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -711,7 +764,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -721,25 +774,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -747,7 +800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -756,7 +809,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -766,21 +819,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -788,7 +841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -796,7 +849,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -804,7 +857,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -812,7 +865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -820,7 +873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -829,8 +882,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" paperSize="9" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -840,24 +893,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -865,7 +918,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -873,7 +926,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -881,24 +934,24 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -908,26 +961,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.875" style="2"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.5" collapsed="true"/>
+    <col min="3" max="4" style="2" width="10.875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="str">
         <f>Conditions!A1</f>
         <v>Conditions</v>
@@ -939,16 +992,34 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="str">
         <f>Conditions!A2</f>
         <v>C1</v>
@@ -972,8 +1043,26 @@
       <c r="G3" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="str">
         <f>Conditions!A3</f>
         <v>C2</v>
@@ -983,10 +1072,10 @@
         <v>b &lt; a+c?</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>25</v>
@@ -997,8 +1086,26 @@
       <c r="G4" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="str">
         <f>Conditions!A4</f>
         <v>C3</v>
@@ -1008,13 +1115,13 @@
         <v>c &lt; a+b?</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>25</v>
@@ -1022,8 +1129,26 @@
       <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="str">
         <f>Conditions!A5</f>
         <v>C4</v>
@@ -1033,13 +1158,13 @@
         <v>a=b?</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>25</v>
@@ -1047,8 +1172,26 @@
       <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="str">
         <f>Conditions!A6</f>
         <v>C5</v>
@@ -1058,13 +1201,13 @@
         <v>a=c?</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>25</v>
@@ -1072,8 +1215,26 @@
       <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="str">
         <f>Conditions!A7</f>
         <v>C6</v>
@@ -1083,13 +1244,13 @@
         <v>b=c?</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>25</v>
@@ -1097,8 +1258,26 @@
       <c r="G8" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="str">
         <f>Actions!A1</f>
         <v>Actions</v>
@@ -1106,8 +1285,14 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="str">
         <f>Actions!A2</f>
         <v>A1</v>
@@ -1119,11 +1304,22 @@
       <c r="C10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="str">
         <f>Actions!A3</f>
         <v>A2</v>
@@ -1132,14 +1328,19 @@
         <f>Actions!B3</f>
         <v>type_of_triangle="Scalene"</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="str">
         <f>Actions!A4</f>
         <v>A3</v>
@@ -1148,44 +1349,73 @@
         <f>Actions!B4</f>
         <v>type_of_triangle="Isosceles"</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="7"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="str">
         <f>Actions!A5</f>
         <v>A4</v>
       </c>
       <c r="B13" t="str">
         <f>Actions!B5</f>
-        <v>Equaliteral</v>
+        <v>type_of_triangle="Equaliteral"</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="str">
         <f>Actions!A6</f>
         <v>A5</v>
       </c>
       <c r="B14" t="str">
         <f>Actions!B6</f>
-        <v>Impossible</v>
+        <v>type_of_triangle="Impossible"</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="H14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="M15" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1195,21 +1425,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.875" style="2"/>
-    <col min="8" max="8" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="2" max="7" style="2" width="10.875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="27.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1217,7 +1447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="B2" s="2" t="str">
         <f>'Decision Table'!A3</f>
         <v>C1</v>
@@ -1227,7 +1457,7 @@
         <v>C2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -1235,11 +1465,26 @@
         <f>'Decision Table'!B3</f>
         <v>a &lt; b+c?</v>
       </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
       <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1247,12 +1492,27 @@
         <f>'Decision Table'!C3</f>
         <v>F</v>
       </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
       <c r="H4" t="str">
         <f>'Decision Table'!B10</f>
         <v>error_message="Not a Triangle"</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1260,9 +1520,261 @@
         <f>'Decision Table'!D3</f>
         <v>T</v>
       </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1272,23 +1784,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.875" style="2"/>
-    <col min="5" max="5" width="17" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.125" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="2"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="2" max="4" style="2" width="10.875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="17.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="15.375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="9" max="9" style="2" width="10.875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row ht="31.5" r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -1305,7 +1817,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="B2" s="2" t="str">
         <f>'Input Variables'!A2</f>
         <v>IV1</v>
@@ -1338,7 +1850,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="B3" s="2" t="str">
         <f>'Input Variables'!B2</f>
         <v>side_a</v>
@@ -1368,19 +1880,19 @@
         <v>error_message</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" paperSize="9" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>